<commit_message>
Updated three eq unweighted
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_6_16.xlsx
+++ b/results/tables/final_tables_6_16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E76EC97-6059-486E-B0D7-0F0D9C1076EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58808D1E-E817-4864-A82D-2D4351381576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14040" yWindow="-18450" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="occupation_numbers" sheetId="11" r:id="rId1"/>
@@ -115,7 +115,7 @@
     <author>tc={134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}</author>
   </authors>
   <commentList>
-    <comment ref="D38" authorId="0" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+    <comment ref="D42" authorId="0" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="165">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -692,6 +692,15 @@
   </si>
   <si>
     <t>0.059***</t>
+  </si>
+  <si>
+    <t>Udpated</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -785,7 +794,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,12 +840,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -943,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1021,7 +1024,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1038,7 +1040,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1047,6 +1049,13 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1080,14 +1089,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1600,7 +1602,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D38" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+  <threadedComment ref="D42" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
     <text>Should I winsorize it?</text>
   </threadedComment>
 </ThreadedComments>
@@ -1708,12 +1710,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1917,7 +1919,7 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -1928,13 +1930,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2012,30 +2014,30 @@
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="55">
         <v>0.31061129999999998</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="55">
         <v>0.20215459999999999</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="55">
         <v>0.180814</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="55">
         <v>0.23334750000000001</v>
       </c>
       <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="71">
+      <c r="B7" s="58">
         <v>156</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="J7" s="30"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -2048,12 +2050,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -2333,16 +2335,16 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="B34" s="55">
+      <c r="B34" s="54">
         <v>156</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="54">
         <v>156</v>
       </c>
-      <c r="D34" s="55">
+      <c r="D34" s="54">
         <v>156</v>
       </c>
     </row>
@@ -2352,12 +2354,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -2457,7 +2459,7 @@
         <v>0.50700000000000001</v>
       </c>
       <c r="D47" s="18">
-        <f t="shared" ref="D47:D60" si="3">+C47-B47</f>
+        <f t="shared" ref="D47:D48" si="3">+C47-B47</f>
         <v>2.200000000000002E-2</v>
       </c>
     </row>
@@ -2495,7 +2497,7 @@
         <v>0.61699999999999999</v>
       </c>
       <c r="D50" s="18">
-        <f t="shared" ref="D50:D60" si="4">+C50-B50</f>
+        <f t="shared" ref="D50:D52" si="4">+C50-B50</f>
         <v>2.4000000000000021E-2</v>
       </c>
     </row>
@@ -2548,7 +2550,7 @@
         <v>0.59899999999999998</v>
       </c>
       <c r="D54" s="18">
-        <f t="shared" ref="D54:D60" si="5">+C54-B54</f>
+        <f t="shared" ref="D54:D56" si="5">+C54-B54</f>
         <v>-3.6000000000000032E-2</v>
       </c>
     </row>
@@ -2636,16 +2638,16 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="54" t="s">
+      <c r="A61" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="55">
+      <c r="B61" s="54">
         <v>62</v>
       </c>
-      <c r="C61" s="55">
+      <c r="C61" s="54">
         <v>62</v>
       </c>
-      <c r="D61" s="55">
+      <c r="D61" s="54">
         <v>62</v>
       </c>
     </row>
@@ -2684,13 +2686,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
@@ -2743,16 +2745,16 @@
       <c r="A6" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="44" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2761,39 +2763,39 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="44" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2802,40 +2804,40 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>-6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>"College+"</f>
         <v>College+</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2844,16 +2846,16 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="45">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
@@ -2928,29 +2930,29 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
     </row>
     <row r="21" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
       <c r="G21" s="32"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3004,19 +3006,19 @@
       <c r="A26" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="45" t="str">
+      <c r="B26" s="44" t="str">
         <f>"0.480***"</f>
         <v>0.480***</v>
       </c>
-      <c r="C26" s="45" t="str">
+      <c r="C26" s="44" t="str">
         <f>"0.644***"</f>
         <v>0.644***</v>
       </c>
-      <c r="D26" s="45" t="str">
+      <c r="D26" s="44" t="str">
         <f>"0.652***"</f>
         <v>0.652***</v>
       </c>
-      <c r="E26" s="45" t="str">
+      <c r="E26" s="44" t="str">
         <f>"0.523***"</f>
         <v>0.523***</v>
       </c>
@@ -3026,46 +3028,46 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B27" s="45" t="str">
+      <c r="B27" s="44" t="str">
         <f>"(0.004)"</f>
         <v>(0.004)</v>
       </c>
-      <c r="C27" s="45" t="str">
+      <c r="C27" s="44" t="str">
         <f>"(0.003)"</f>
         <v>(0.003)</v>
       </c>
-      <c r="D27" s="45" t="str">
+      <c r="D27" s="44" t="str">
         <f>"(0.004)"</f>
         <v>(0.004)</v>
       </c>
-      <c r="E27" s="45" t="str">
+      <c r="E27" s="44" t="str">
         <f>"(0.003)"</f>
         <v>(0.003)</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="45" t="str">
+      <c r="B29" s="44" t="str">
         <f>"-0.018**"</f>
         <v>-0.018**</v>
       </c>
-      <c r="C29" s="45" t="str">
+      <c r="C29" s="44" t="str">
         <f>"0.015***"</f>
         <v>0.015***</v>
       </c>
-      <c r="D29" s="45" t="str">
+      <c r="D29" s="44" t="str">
         <f>"0.009"</f>
         <v>0.009</v>
       </c>
-      <c r="E29" s="45" t="str">
+      <c r="E29" s="44" t="str">
         <f>"0.025***"</f>
         <v>0.025***</v>
       </c>
@@ -3075,47 +3077,47 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B30" s="45" t="str">
+      <c r="B30" s="44" t="str">
         <f>"(0.008)"</f>
         <v>(0.008)</v>
       </c>
-      <c r="C30" s="45" t="str">
+      <c r="C30" s="44" t="str">
         <f>"(0.005)"</f>
         <v>(0.005)</v>
       </c>
-      <c r="D30" s="45" t="str">
+      <c r="D30" s="44" t="str">
         <f>"(0.007)"</f>
         <v>(0.007)</v>
       </c>
-      <c r="E30" s="45" t="str">
+      <c r="E30" s="44" t="str">
         <f>"(0.006)"</f>
         <v>(0.006)</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>"College+"</f>
         <v>College+</v>
       </c>
-      <c r="B32" s="45" t="str">
+      <c r="B32" s="44" t="str">
         <f>"-0.079***"</f>
         <v>-0.079***</v>
       </c>
-      <c r="C32" s="45" t="str">
+      <c r="C32" s="44" t="str">
         <f>"0.043***"</f>
         <v>0.043***</v>
       </c>
-      <c r="D32" s="45" t="str">
+      <c r="D32" s="44" t="str">
         <f>"0.033***"</f>
         <v>0.033***</v>
       </c>
-      <c r="E32" s="45" t="str">
+      <c r="E32" s="44" t="str">
         <f>"0.058***"</f>
         <v>0.058***</v>
       </c>
@@ -3125,19 +3127,19 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B33" s="45" t="str">
+      <c r="B33" s="44" t="str">
         <f>"(0.010)"</f>
         <v>(0.010)</v>
       </c>
-      <c r="C33" s="45" t="str">
+      <c r="C33" s="44" t="str">
         <f>"(0.006)"</f>
         <v>(0.006)</v>
       </c>
-      <c r="D33" s="45" t="str">
+      <c r="D33" s="44" t="str">
         <f>"(0.007)"</f>
         <v>(0.007)</v>
       </c>
-      <c r="E33" s="45" t="str">
+      <c r="E33" s="44" t="str">
         <f>"(0.006)"</f>
         <v>(0.006)</v>
       </c>
@@ -3213,13 +3215,13 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
     </row>
     <row r="41" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -3259,7 +3261,7 @@
       <c r="C3" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>212</v>
       </c>
     </row>
@@ -3272,10 +3274,10 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="42">
         <v>9</v>
       </c>
     </row>
@@ -3295,7 +3297,7 @@
       <c r="C9" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="44"/>
+      <c r="D9" s="43"/>
       <c r="E9" s="25" t="s">
         <v>138</v>
       </c>
@@ -3564,36 +3566,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
       <c r="AC1" s="32"/>
     </row>
     <row r="2" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4042,10 +4044,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4055,24 +4057,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="41"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="70"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -4189,668 +4188,695 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="69" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="69" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="69" t="s">
-        <v>23</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="63" t="s">
+      <c r="B10" s="4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="41"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G12" s="62" t="s">
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="70"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G13" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="10" t="s">
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I14" s="8" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="9">
-        <v>0.243728048163528</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0.30639338586139098</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.94781940223736805</v>
-      </c>
-      <c r="E14" s="9">
-        <v>6.8997895402579598E-2</v>
-      </c>
-      <c r="G14" s="18">
-        <f t="shared" ref="G14:I16" si="2">+C14/$B14</f>
-        <v>1.2571117200914768</v>
-      </c>
-      <c r="H14" s="18">
-        <f t="shared" si="2"/>
-        <v>3.888840079667129</v>
-      </c>
-      <c r="I14" s="18">
-        <f t="shared" si="2"/>
-        <v>0.28309378392217638</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B15" s="9">
-        <v>0.243728048163528</v>
+        <v>0.23048887991556499</v>
       </c>
       <c r="C15" s="9">
-        <v>0.649996885772121</v>
+        <v>0.52304380173648501</v>
       </c>
       <c r="D15" s="9">
-        <v>0.62369711452125598</v>
+        <v>0.78124635093675499</v>
       </c>
       <c r="E15" s="9">
-        <v>1.64025266039926E-2</v>
+        <v>1.8461253258520001E-2</v>
       </c>
       <c r="G15" s="18">
-        <f t="shared" si="2"/>
-        <v>2.6668940676700825</v>
+        <f t="shared" ref="G15:I17" si="2">+C15/$B15</f>
+        <v>2.2692799840412765</v>
       </c>
       <c r="H15" s="18">
         <f t="shared" si="2"/>
-        <v>2.5589878523246115</v>
+        <v>3.389518623297354</v>
       </c>
       <c r="I15" s="18">
         <f t="shared" si="2"/>
-        <v>6.7298477658129088E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="20">
-        <v>0.243728048163528</v>
-      </c>
-      <c r="C16" s="20">
-        <v>0.80900159771423297</v>
-      </c>
-      <c r="D16" s="20">
-        <v>0.43380470102729102</v>
-      </c>
-      <c r="E16" s="20">
-        <v>1.04049831254575E-2</v>
+        <v>8.0096069126124061E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.23048887991556499</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.555574885853796</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.72666774603677697</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1.89933711389241E-2</v>
       </c>
       <c r="G16" s="18">
         <f t="shared" si="2"/>
-        <v>3.3192798441131313</v>
+        <v>2.4104194790539126</v>
       </c>
       <c r="H16" s="18">
         <f t="shared" si="2"/>
-        <v>1.7798718871134278</v>
+        <v>3.1527236641653915</v>
       </c>
       <c r="I16" s="18">
         <f t="shared" si="2"/>
-        <v>4.2690954955156957E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="69" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="69" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="69" t="s">
-        <v>23</v>
+        <v>8.2404717945099751E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="20">
+        <v>0.23048887991556499</v>
+      </c>
+      <c r="C17" s="20">
+        <v>0.91092319378507403</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0.32785505366336998</v>
+      </c>
+      <c r="E17" s="20">
+        <v>2.0726558117770001E-2</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" si="2"/>
+        <v>3.952135105688277</v>
+      </c>
+      <c r="H17" s="18">
+        <f t="shared" si="2"/>
+        <v>1.4224332808744315</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="2"/>
+        <v>8.992433008205325E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-    </row>
-    <row r="21" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="63" t="s">
+      <c r="B21" s="1">
+        <v>62</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="41"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G22" s="62" t="s">
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="70"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G24" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="10" t="s">
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I25" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B26" s="9">
         <v>0.28653203408786099</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C26" s="9">
         <v>0.432813593737364</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D26" s="9">
         <v>0.72863646579924202</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E26" s="9">
         <v>0.13590170492659701</v>
       </c>
-      <c r="G24" s="18">
-        <f t="shared" ref="G24:I26" si="3">+C24/$B24</f>
+      <c r="G26" s="18">
+        <f t="shared" ref="G26:I28" si="3">+C26/$B26</f>
         <v>1.5105242773820111</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H26" s="18">
         <f t="shared" si="3"/>
         <v>2.5429494057052482</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I26" s="18">
         <f t="shared" si="3"/>
         <v>0.47429846843904605</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B27" s="9">
         <v>0.276932075864669</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C27" s="9">
         <v>0.57770093297611302</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D27" s="9">
         <v>0.59045981810458203</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E27" s="9">
         <v>0.11649908855437099</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G27" s="18">
         <f t="shared" si="3"/>
         <v>2.0860744685221064</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H27" s="18">
         <f t="shared" si="3"/>
         <v>2.1321467232027236</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I27" s="18">
         <f t="shared" si="3"/>
         <v>0.42067748270265992</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="19" t="s">
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B28" s="20">
         <v>0.26284326769114302</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C28" s="20">
         <v>0.69281313851899595</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D28" s="20">
         <v>0.46538756699114298</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E28" s="20">
         <v>8.4193690103555402E-2</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G28" s="18">
         <f t="shared" si="3"/>
         <v>2.635841292815968</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H28" s="18">
         <f t="shared" si="3"/>
         <v>1.7705896410403859</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I28" s="18">
         <f t="shared" si="3"/>
         <v>0.32031899026034083</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="69" t="s">
+      <c r="B31" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="69" t="s">
+      <c r="C31" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="69" t="s">
+      <c r="D31" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="69" t="s">
+      <c r="E31" s="57" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A31" s="63" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="41"/>
-    </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G32" s="62" t="s">
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="70"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G35" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="62"/>
-      <c r="I32" s="62"/>
-    </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="10" t="s">
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G36" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H36" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I36" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B37" s="9">
         <v>0.27694137299481097</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C37" s="9">
         <v>0.42839703824389602</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D37" s="9">
         <v>0.73221967455815895</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E37" s="9">
         <v>0.14522662046094101</v>
       </c>
-      <c r="G34" s="18">
-        <f t="shared" ref="G34:G36" si="4">+C34/$B34</f>
+      <c r="G37" s="18">
+        <f t="shared" ref="G37:G39" si="4">+C37/$B37</f>
         <v>1.5468871032567708</v>
       </c>
-      <c r="H34" s="18">
-        <f t="shared" ref="H34:H36" si="5">+D34/$B34</f>
+      <c r="H37" s="18">
+        <f t="shared" ref="H37:H39" si="5">+D37/$B37</f>
         <v>2.6439519189206826</v>
       </c>
-      <c r="I34" s="18">
-        <f t="shared" ref="I34:I36" si="6">+E34/$B34</f>
+      <c r="I37" s="18">
+        <f t="shared" ref="I37:I39" si="6">+E37/$B37</f>
         <v>0.52439481645691888</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B38" s="9">
         <v>0.27694137299481097</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C38" s="9">
         <v>0.57228268588881703</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D38" s="9">
         <v>0.58926620862447998</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E38" s="9">
         <v>0.124157838755312</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G38" s="18">
         <f t="shared" si="4"/>
         <v>2.0664398377902886</v>
       </c>
-      <c r="H35" s="18">
+      <c r="H38" s="18">
         <f t="shared" si="5"/>
         <v>2.127765173734157</v>
       </c>
-      <c r="I35" s="18">
+      <c r="I38" s="18">
         <f t="shared" si="6"/>
         <v>0.44831813106392859</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="19" t="s">
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B39" s="20">
         <v>0.27694137299481097</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C39" s="20">
         <v>0.68823758898142895</v>
       </c>
-      <c r="D36" s="20">
+      <c r="D39" s="20">
         <v>0.45037536250430998</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E39" s="20">
         <v>9.6539983270205507E-2</v>
       </c>
-      <c r="G36" s="18">
+      <c r="G39" s="18">
         <f t="shared" si="4"/>
         <v>2.485138213690897</v>
       </c>
-      <c r="H36" s="18">
+      <c r="H39" s="18">
         <f t="shared" si="5"/>
         <v>1.626248030888287</v>
       </c>
-      <c r="I36" s="18">
+      <c r="I39" s="18">
         <f t="shared" si="6"/>
         <v>0.34859357497304805</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="69" t="s">
+      <c r="B42" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="69" t="s">
+      <c r="C42" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="69" t="s">
+      <c r="D42" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="69" t="s">
+      <c r="E42" s="57" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B40" s="70"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-    </row>
-    <row r="41" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="63" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="63"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="41"/>
-    </row>
-    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G42" s="62" t="s">
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="70"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G46" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-    </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="10" t="s">
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B47" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C47" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D47" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E47" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G47" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H47" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="I47" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>115</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B48" s="9">
         <v>0.28183327657601598</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C48" s="9">
         <v>0.451604949468082</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D48" s="9">
         <v>0.72629296980184699</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E48" s="9">
         <v>0.126547412046842</v>
       </c>
-      <c r="G44" s="18">
-        <f t="shared" ref="G44:G46" si="7">+C44/$B44</f>
+      <c r="G48" s="18">
+        <f t="shared" ref="G48:G50" si="7">+C48/$B48</f>
         <v>1.6023833486045969</v>
       </c>
-      <c r="H44" s="18">
-        <f t="shared" ref="H44:H46" si="8">+D44/$B44</f>
+      <c r="H48" s="18">
+        <f t="shared" ref="H48:H50" si="8">+D48/$B48</f>
         <v>2.5770305714980095</v>
       </c>
-      <c r="I44" s="18">
-        <f t="shared" ref="I44:I46" si="9">+E44/$B44</f>
+      <c r="I48" s="18">
+        <f t="shared" ref="I48:I50" si="9">+E48/$B48</f>
         <v>0.44901515386778562</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B49" s="9">
         <v>0.28183327657601598</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C49" s="9">
         <v>0.57312702766578705</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D49" s="9">
         <v>0.58547428345952901</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E49" s="9">
         <v>0.126990845337904</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G49" s="18">
         <f t="shared" si="7"/>
         <v>2.033567627743218</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H49" s="18">
         <f t="shared" si="8"/>
         <v>2.0773781243025611</v>
       </c>
-      <c r="I45" s="18">
+      <c r="I49" s="18">
         <f t="shared" si="9"/>
         <v>0.4505885425621558</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="19" t="s">
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="20">
+      <c r="B50" s="20">
         <v>0.28183327657601598</v>
       </c>
-      <c r="C46" s="20">
+      <c r="C50" s="20">
         <v>0.73026257014047502</v>
       </c>
-      <c r="D46" s="20">
+      <c r="D50" s="20">
         <v>0.395929548503758</v>
       </c>
-      <c r="E46" s="20">
+      <c r="E50" s="20">
         <v>0.114035512352252</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G50" s="18">
         <f t="shared" si="7"/>
         <v>2.5911154957016187</v>
       </c>
-      <c r="H46" s="18">
+      <c r="H50" s="18">
         <f t="shared" si="8"/>
         <v>1.4048360552518646</v>
       </c>
-      <c r="I46" s="18">
+      <c r="I50" s="18">
         <f t="shared" si="9"/>
         <v>0.40462046830546772</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="69" t="s">
+      <c r="B53" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="69" t="s">
+      <c r="C53" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="69" t="s">
+      <c r="D53" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="E48" s="69" t="s">
+      <c r="E53" s="57" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="G46:I46"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G24:I24"/>
   </mergeCells>
-  <conditionalFormatting sqref="G14:G16">
+  <conditionalFormatting sqref="G15:G17">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -4860,7 +4886,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H16">
+  <conditionalFormatting sqref="H15:H17">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -4870,7 +4896,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I16">
+  <conditionalFormatting sqref="I15:I17">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -4910,7 +4936,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34:G36">
+  <conditionalFormatting sqref="G37:G39">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -4920,7 +4946,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34:H36">
+  <conditionalFormatting sqref="H37:H39">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -4930,7 +4956,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I34:I36">
+  <conditionalFormatting sqref="I37:I39">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -4940,7 +4966,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44:G46">
+  <conditionalFormatting sqref="G48:G50">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -4950,7 +4976,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44:H46">
+  <conditionalFormatting sqref="H48:H50">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -4960,7 +4986,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44:I46">
+  <conditionalFormatting sqref="I48:I50">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4970,7 +4996,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:G26">
+  <conditionalFormatting sqref="G26:G28">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -4980,7 +5006,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24:H26">
+  <conditionalFormatting sqref="H26:H28">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4990,7 +5016,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24:I26">
+  <conditionalFormatting sqref="I26:I28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5024,24 +5050,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
       <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -5237,7 +5263,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="K1" s="52"/>
+      <c r="K1" s="51"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -5260,7 +5286,7 @@
       <c r="B3" s="35"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="42"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="10" t="s">
         <v>84</v>
       </c>
@@ -5275,7 +5301,7 @@
       <c r="E5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="49">
+      <c r="F5" s="48">
         <v>93</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -5295,7 +5321,7 @@
       <c r="E6" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="50">
+      <c r="F6" s="49">
         <v>93</v>
       </c>
       <c r="H6" t="s">
@@ -5385,7 +5411,7 @@
       <c r="E13" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F13" s="50">
         <v>89.044470000000004</v>
       </c>
     </row>
@@ -5398,10 +5424,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="47">
+      <c r="B15" s="46">
         <v>0.99</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="47">
         <v>789.47889999999995</v>
       </c>
     </row>
@@ -5425,7 +5451,7 @@
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="42"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="10" t="s">
         <v>84</v>
       </c>
@@ -5501,10 +5527,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="47">
+      <c r="B30" s="46">
         <v>0.99</v>
       </c>
-      <c r="C30" s="48">
+      <c r="C30" s="47">
         <v>789.47889999999995</v>
       </c>
     </row>
@@ -5532,35 +5558,35 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66" t="s">
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="67" t="s">
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="67"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="69"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B3" t="s">

</xml_diff>